<commit_message>
adding subphyllum in TABLE S3 and removing background color in xlsx files
</commit_message>
<xml_diff>
--- a/Data/TABLE_S1_COM1.xlsx
+++ b/Data/TABLE_S1_COM1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012D6D6F-D5E1-47C5-9288-F468EA17E562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2E8F79-AEC9-4CC1-A8CE-CAF6E0E5A6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{89A25F2E-5CBE-B84E-9E40-85B2FEE01AB5}"/>
   </bookViews>
@@ -1343,7 +1343,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1352,31 +1352,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1445,7 +1421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1456,150 +1432,102 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1917,1197 +1845,1228 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63F2132-EC0E-EB4E-B287-2A6C5ABCEA97}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="4" customWidth="1"/>
     <col min="2" max="5" width="3.796875" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.19921875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" style="10"/>
-    <col min="8" max="8" width="13.296875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="39.796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" style="5"/>
+    <col min="8" max="8" width="13.296875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="39.796875" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.796875" style="1"/>
     <col min="12" max="12" width="65.296875" style="3" customWidth="1"/>
     <col min="13" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="52"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18">
+      <c r="B3" s="13"/>
+      <c r="C3" s="35">
         <v>2</v>
       </c>
-      <c r="D3" s="18">
-        <v>1</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="D3" s="35">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="1">
-        <v>100</v>
-      </c>
-      <c r="K3" s="1">
-        <v>100</v>
-      </c>
-      <c r="L3" s="23" t="s">
+      <c r="J3" s="14">
+        <v>100</v>
+      </c>
+      <c r="K3" s="14">
+        <v>100</v>
+      </c>
+      <c r="L3" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18">
+      <c r="B4" s="13"/>
+      <c r="C4" s="35">
         <v>2</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="1">
-        <v>100</v>
-      </c>
-      <c r="K4" s="1">
-        <v>100</v>
-      </c>
-      <c r="L4" s="23" t="s">
+      <c r="J4" s="14">
+        <v>100</v>
+      </c>
+      <c r="K4" s="14">
+        <v>100</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="19">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="35">
+        <v>1</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="13">
-        <v>100</v>
-      </c>
-      <c r="K5" s="14">
-        <v>100</v>
-      </c>
-      <c r="L5" s="23" t="s">
+      <c r="J5" s="23">
+        <v>100</v>
+      </c>
+      <c r="K5" s="24">
+        <v>100</v>
+      </c>
+      <c r="L5" s="15" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="19">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="35">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="16">
-        <v>100</v>
-      </c>
-      <c r="K6" s="30">
+      <c r="J6" s="18">
+        <v>100</v>
+      </c>
+      <c r="K6" s="26">
         <v>99</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="15" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="19">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="35">
         <v>2</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="18"/>
+      <c r="H7" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="J7" s="16">
-        <v>100</v>
-      </c>
-      <c r="K7" s="30">
-        <v>100</v>
-      </c>
-      <c r="L7" s="23" t="s">
+      <c r="J7" s="18">
+        <v>100</v>
+      </c>
+      <c r="K7" s="26">
+        <v>100</v>
+      </c>
+      <c r="L7" s="15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="46">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="35" t="s">
+      <c r="B8" s="35">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="23">
         <v>97.32</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="24">
         <v>81</v>
       </c>
-      <c r="L8" s="48" t="s">
+      <c r="L8" s="15" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="19">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="35">
+        <v>1</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="23">
         <v>99.58</v>
       </c>
-      <c r="K9" s="14">
-        <v>100</v>
-      </c>
-      <c r="L9" s="23" t="s">
+      <c r="K9" s="24">
+        <v>100</v>
+      </c>
+      <c r="L9" s="15" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="19">
-        <v>1</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="35">
+        <v>1</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="13">
-        <v>100</v>
-      </c>
-      <c r="K10" s="14">
-        <v>100</v>
-      </c>
-      <c r="L10" s="23" t="s">
+      <c r="J10" s="23">
+        <v>100</v>
+      </c>
+      <c r="K10" s="24">
+        <v>100</v>
+      </c>
+      <c r="L10" s="15" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="20">
-        <v>1</v>
-      </c>
-      <c r="C11" s="20">
-        <v>1</v>
-      </c>
-      <c r="D11" s="20">
-        <v>1</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="B11" s="36">
+        <v>1</v>
+      </c>
+      <c r="C11" s="36">
+        <v>1</v>
+      </c>
+      <c r="D11" s="36">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="13">
-        <v>100</v>
-      </c>
-      <c r="K11" s="14">
-        <v>100</v>
-      </c>
-      <c r="L11" s="23" t="s">
+      <c r="J11" s="23">
+        <v>100</v>
+      </c>
+      <c r="K11" s="24">
+        <v>100</v>
+      </c>
+      <c r="L11" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+    <row r="12" spans="1:12" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="46">
-        <v>1</v>
-      </c>
-      <c r="D12" s="46">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="35" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="35">
+        <v>1</v>
+      </c>
+      <c r="D12" s="35">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="J12" s="36">
-        <v>100</v>
-      </c>
-      <c r="K12" s="42">
-        <v>100</v>
-      </c>
-      <c r="L12" s="48" t="s">
+      <c r="J12" s="18">
+        <v>100</v>
+      </c>
+      <c r="K12" s="26">
+        <v>100</v>
+      </c>
+      <c r="L12" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="34" t="s">
+    <row r="13" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="47">
-        <v>1</v>
-      </c>
-      <c r="D13" s="46">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="35" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="36">
+        <v>1</v>
+      </c>
+      <c r="D13" s="35">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="38">
+      <c r="J13" s="23">
         <v>99.31</v>
       </c>
-      <c r="K13" s="39">
-        <v>100</v>
-      </c>
-      <c r="L13" s="48" t="s">
+      <c r="K13" s="24">
+        <v>100</v>
+      </c>
+      <c r="L13" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+    <row r="14" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="47">
-        <v>1</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="43" t="s">
+      <c r="B14" s="36">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="38">
-        <v>100</v>
-      </c>
-      <c r="K14" s="39">
+      <c r="J14" s="23">
+        <v>100</v>
+      </c>
+      <c r="K14" s="24">
         <v>99</v>
       </c>
-      <c r="L14" s="48" t="s">
+      <c r="L14" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="47">
-        <v>1</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="43" t="s">
+      <c r="B15" s="36">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="J15" s="38">
+      <c r="J15" s="23">
         <v>99.65</v>
       </c>
-      <c r="K15" s="39">
+      <c r="K15" s="24">
         <v>99</v>
       </c>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="44" t="s">
+    <row r="16" spans="1:12" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="46">
-        <v>1</v>
-      </c>
-      <c r="F16" s="35" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="35">
+        <v>1</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="J16" s="36">
-        <v>100</v>
-      </c>
-      <c r="K16" s="42">
-        <v>100</v>
-      </c>
-      <c r="L16" s="48" t="s">
+      <c r="J16" s="18">
+        <v>100</v>
+      </c>
+      <c r="K16" s="26">
+        <v>100</v>
+      </c>
+      <c r="L16" s="15" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="20">
-        <v>1</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="E17" s="19">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="B17" s="36">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="35">
+        <v>1</v>
+      </c>
+      <c r="F17" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="23">
         <v>99.82</v>
       </c>
-      <c r="K17" s="14">
-        <v>100</v>
-      </c>
-      <c r="L17" s="23" t="s">
+      <c r="K17" s="24">
+        <v>100</v>
+      </c>
+      <c r="L17" s="15" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="C18" s="19">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="35">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="23">
         <v>99.82</v>
       </c>
-      <c r="K18" s="14">
-        <v>100</v>
-      </c>
-      <c r="L18" s="23" t="s">
+      <c r="K18" s="24">
+        <v>100</v>
+      </c>
+      <c r="L18" s="15" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="18">
-        <v>1</v>
-      </c>
-      <c r="F19" s="23" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="35">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="K19" s="1">
-        <v>100</v>
-      </c>
-      <c r="L19" s="23" t="s">
+      <c r="K19" s="14">
+        <v>100</v>
+      </c>
+      <c r="L19" s="15" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="18">
-        <v>1</v>
-      </c>
-      <c r="F20" s="23" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="35">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="K20" s="1">
-        <v>100</v>
-      </c>
-      <c r="L20" s="23" t="s">
+      <c r="K20" s="14">
+        <v>100</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="20">
-        <v>1</v>
-      </c>
-      <c r="C21" s="20">
-        <v>1</v>
-      </c>
-      <c r="D21" s="19">
-        <v>1</v>
-      </c>
-      <c r="E21" s="19">
-        <v>1</v>
-      </c>
-      <c r="F21" s="11" t="s">
+      <c r="B21" s="36">
+        <v>1</v>
+      </c>
+      <c r="C21" s="36">
+        <v>1</v>
+      </c>
+      <c r="D21" s="35">
+        <v>1</v>
+      </c>
+      <c r="E21" s="35">
+        <v>1</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="J21" s="16">
-        <v>100</v>
-      </c>
-      <c r="K21" s="30">
-        <v>100</v>
-      </c>
-      <c r="L21" s="23" t="s">
+      <c r="J21" s="18">
+        <v>100</v>
+      </c>
+      <c r="K21" s="26">
+        <v>100</v>
+      </c>
+      <c r="L21" s="15" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="E22" s="19">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="35">
+        <v>1</v>
+      </c>
+      <c r="F22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J22" s="16">
-        <v>100</v>
-      </c>
-      <c r="K22" s="30">
-        <v>100</v>
-      </c>
-      <c r="L22" s="23" t="s">
+      <c r="J22" s="18">
+        <v>100</v>
+      </c>
+      <c r="K22" s="26">
+        <v>100</v>
+      </c>
+      <c r="L22" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="40" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49" t="s">
+    <row r="23" spans="1:12" s="34" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B23" s="47">
+      <c r="B23" s="36">
         <v>4</v>
       </c>
-      <c r="C23" s="47">
+      <c r="C23" s="36">
         <v>13</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="35">
         <v>7</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="35" t="s">
+      <c r="E23" s="14"/>
+      <c r="F23" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="G23" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="37" t="s">
+      <c r="H23" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="I23" s="36" t="s">
+      <c r="I23" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="36">
-        <v>100</v>
-      </c>
-      <c r="K23" s="42">
-        <v>100</v>
-      </c>
-      <c r="L23" s="48" t="s">
+      <c r="J23" s="18">
+        <v>100</v>
+      </c>
+      <c r="K23" s="26">
+        <v>100</v>
+      </c>
+      <c r="L23" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="41" t="s">
+    <row r="24" spans="1:12" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="47">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="43" t="s">
+      <c r="B24" s="36">
+        <v>1</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="36" t="s">
+      <c r="G24" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="I24" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="J24" s="38">
-        <v>100</v>
-      </c>
-      <c r="K24" s="39">
-        <v>100</v>
-      </c>
-      <c r="L24" s="48" t="s">
+      <c r="J24" s="23">
+        <v>100</v>
+      </c>
+      <c r="K24" s="24">
+        <v>100</v>
+      </c>
+      <c r="L24" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="40" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+    <row r="25" spans="1:12" s="34" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="47">
+      <c r="B25" s="13"/>
+      <c r="C25" s="36">
         <v>4</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="46">
-        <v>1</v>
-      </c>
-      <c r="F25" s="43" t="s">
+      <c r="D25" s="14"/>
+      <c r="E25" s="35">
+        <v>1</v>
+      </c>
+      <c r="F25" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="37" t="s">
+      <c r="H25" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="I25" s="38" t="s">
+      <c r="I25" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="J25" s="38">
+      <c r="J25" s="23">
         <v>98.62</v>
       </c>
-      <c r="K25" s="39">
-        <v>100</v>
-      </c>
-      <c r="L25" s="48" t="s">
+      <c r="K25" s="24">
+        <v>100</v>
+      </c>
+      <c r="L25" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="40" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="34" t="s">
+    <row r="26" spans="1:12" s="34" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="47">
+      <c r="B26" s="13"/>
+      <c r="C26" s="36">
         <v>2</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="43" t="s">
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="37" t="s">
+      <c r="H26" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="J26" s="38">
+      <c r="J26" s="23">
         <v>99.53</v>
       </c>
-      <c r="K26" s="39">
-        <v>100</v>
-      </c>
-      <c r="L26" s="48" t="s">
+      <c r="K26" s="24">
+        <v>100</v>
+      </c>
+      <c r="L26" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="40" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="34" t="s">
+    <row r="27" spans="1:12" s="34" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="47">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="43" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="36">
+        <v>1</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="37" t="s">
+      <c r="H27" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="I27" s="38" t="s">
+      <c r="I27" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="J27" s="38">
+      <c r="J27" s="23">
         <v>98.18</v>
       </c>
-      <c r="K27" s="39">
-        <v>100</v>
-      </c>
-      <c r="L27" s="48" t="s">
+      <c r="K27" s="24">
+        <v>100</v>
+      </c>
+      <c r="L27" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="41" t="s">
+    <row r="28" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="46">
+      <c r="B28" s="35">
         <v>2</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="35" t="s">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="37" t="s">
+      <c r="H28" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I28" s="36" t="s">
+      <c r="I28" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J28" s="38">
-        <v>100</v>
-      </c>
-      <c r="K28" s="39">
-        <v>100</v>
-      </c>
-      <c r="L28" s="48" t="s">
+      <c r="J28" s="23">
+        <v>100</v>
+      </c>
+      <c r="K28" s="24">
+        <v>100</v>
+      </c>
+      <c r="L28" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="40" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
+    <row r="29" spans="1:12" s="34" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="47">
-        <v>1</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="35" t="s">
+      <c r="B29" s="36">
+        <v>1</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="G29" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H29" s="37" t="s">
+      <c r="H29" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I29" s="36" t="s">
+      <c r="I29" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J29" s="38">
+      <c r="J29" s="23">
         <v>99.24</v>
       </c>
-      <c r="K29" s="39">
-        <v>100</v>
-      </c>
-      <c r="L29" s="48" t="s">
+      <c r="K29" s="24">
+        <v>100</v>
+      </c>
+      <c r="L29" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34" t="s">
+    <row r="30" spans="1:12" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="47">
-        <v>1</v>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="35" t="s">
+      <c r="B30" s="36">
+        <v>1</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="37" t="s">
+      <c r="H30" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="I30" s="36" t="s">
+      <c r="I30" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J30" s="38">
+      <c r="J30" s="23">
         <v>99.75</v>
       </c>
-      <c r="K30" s="39">
-        <v>100</v>
-      </c>
-      <c r="L30" s="48" t="s">
+      <c r="K30" s="24">
+        <v>100</v>
+      </c>
+      <c r="L30" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
+    <row r="31" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="47">
+      <c r="B31" s="13"/>
+      <c r="C31" s="36">
         <v>6</v>
       </c>
-      <c r="D31" s="46">
+      <c r="D31" s="35">
         <v>2</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="43" t="s">
+      <c r="E31" s="14"/>
+      <c r="F31" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="36" t="s">
+      <c r="G31" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H31" s="37" t="s">
+      <c r="H31" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I31" s="38" t="s">
+      <c r="I31" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="J31" s="38">
-        <v>100</v>
-      </c>
-      <c r="K31" s="39">
-        <v>100</v>
-      </c>
-      <c r="L31" s="48" t="s">
+      <c r="J31" s="23">
+        <v>100</v>
+      </c>
+      <c r="K31" s="24">
+        <v>100</v>
+      </c>
+      <c r="L31" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+    <row r="32" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="47">
-        <v>1</v>
-      </c>
-      <c r="D32" s="46">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="43" t="s">
+      <c r="B32" s="13"/>
+      <c r="C32" s="36">
+        <v>1</v>
+      </c>
+      <c r="D32" s="35">
+        <v>1</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G32" s="36" t="s">
+      <c r="G32" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H32" s="37" t="s">
+      <c r="H32" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="I32" s="38" t="s">
+      <c r="I32" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="J32" s="38">
-        <v>100</v>
-      </c>
-      <c r="K32" s="39">
-        <v>100</v>
-      </c>
-      <c r="L32" s="48" t="s">
+      <c r="J32" s="23">
+        <v>100</v>
+      </c>
+      <c r="K32" s="24">
+        <v>100</v>
+      </c>
+      <c r="L32" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
+    <row r="33" spans="1:12" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="47">
-        <v>1</v>
-      </c>
-      <c r="D33" s="46">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="43" t="s">
+      <c r="B33" s="13"/>
+      <c r="C33" s="36">
+        <v>1</v>
+      </c>
+      <c r="D33" s="35">
+        <v>1</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="36" t="s">
+      <c r="G33" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H33" s="37" t="s">
+      <c r="H33" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="I33" s="38" t="s">
+      <c r="I33" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="J33" s="38">
+      <c r="J33" s="23">
         <v>99.46</v>
       </c>
-      <c r="K33" s="39">
-        <v>100</v>
-      </c>
-      <c r="L33" s="48" t="s">
+      <c r="K33" s="24">
+        <v>100</v>
+      </c>
+      <c r="L33" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:12" s="34" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="47">
-        <v>1</v>
-      </c>
-      <c r="D34" s="46">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="43" t="s">
+      <c r="B34" s="13"/>
+      <c r="C34" s="36">
+        <v>1</v>
+      </c>
+      <c r="D34" s="35">
+        <v>1</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G34" s="36" t="s">
+      <c r="G34" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="37" t="s">
+      <c r="H34" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="I34" s="38" t="s">
+      <c r="I34" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="J34" s="38">
+      <c r="J34" s="23">
         <v>99.64</v>
       </c>
-      <c r="K34" s="39">
-        <v>100</v>
-      </c>
-      <c r="L34" s="48" t="s">
+      <c r="K34" s="24">
+        <v>100</v>
+      </c>
+      <c r="L34" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="40" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34" t="s">
+    <row r="35" spans="1:12" s="34" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="47">
-        <v>1</v>
-      </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="43" t="s">
+      <c r="B35" s="36">
+        <v>1</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="36" t="s">
+      <c r="G35" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="H35" s="37" t="s">
+      <c r="H35" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="I35" s="38" t="s">
+      <c r="I35" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="J35" s="38">
+      <c r="J35" s="23">
         <v>99.46</v>
       </c>
-      <c r="K35" s="39">
-        <v>100</v>
-      </c>
-      <c r="L35" s="48" t="s">
+      <c r="K35" s="24">
+        <v>100</v>
+      </c>
+      <c r="L35" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="40" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34" t="s">
+    <row r="36" spans="1:12" s="34" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="47">
+      <c r="B36" s="13"/>
+      <c r="C36" s="36">
         <v>2</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="43" t="s">
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="G36" s="36" t="s">
+      <c r="G36" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H36" s="37" t="s">
+      <c r="H36" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="I36" s="36" t="s">
+      <c r="I36" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J36" s="38">
-        <v>100</v>
-      </c>
-      <c r="K36" s="39">
-        <v>100</v>
-      </c>
-      <c r="L36" s="48" t="s">
+      <c r="J36" s="23">
+        <v>100</v>
+      </c>
+      <c r="K36" s="24">
+        <v>100</v>
+      </c>
+      <c r="L36" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="47">
-        <v>1</v>
-      </c>
-      <c r="C37" s="47">
+    <row r="37" spans="1:12" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="36">
+        <v>1</v>
+      </c>
+      <c r="C37" s="36">
         <v>2</v>
       </c>
-      <c r="D37" s="46">
+      <c r="D37" s="35">
         <v>2</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="43" t="s">
+      <c r="E37" s="14"/>
+      <c r="F37" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="G37" s="36" t="s">
+      <c r="G37" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H37" s="37" t="s">
+      <c r="H37" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="I37" s="38" t="s">
+      <c r="I37" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="J37" s="38">
-        <v>100</v>
-      </c>
-      <c r="K37" s="39">
-        <v>100</v>
-      </c>
-      <c r="L37" s="48" t="s">
+      <c r="J37" s="23">
+        <v>100</v>
+      </c>
+      <c r="K37" s="24">
+        <v>100</v>
+      </c>
+      <c r="L37" s="15" t="s">
         <v>179</v>
       </c>
     </row>

</xml_diff>